<commit_message>
Update sample table for input
</commit_message>
<xml_diff>
--- a/inputs/tsi_seroconvertor_beehive.xlsx
+++ b/inputs/tsi_seroconvertor_beehive.xlsx
@@ -8334,7 +8334,7 @@
         <v>85</v>
       </c>
       <c r="N62" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="O62" t="s">
         <v>35</v>
@@ -10732,7 +10732,7 @@
         <v>97</v>
       </c>
       <c r="N91" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="O91" t="s">
         <v>35</v>
@@ -11302,7 +11302,7 @@
         <v>96.75</v>
       </c>
       <c r="N98" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="O98" t="s">
         <v>35</v>

</xml_diff>